<commit_message>
Unfinished fileimports for products and third party urls. Main issue was getting right amounts of variants created with the right property types and values.
</commit_message>
<xml_diff>
--- a/spree_product_template.xlsx
+++ b/spree_product_template.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+  <si>
+    <t>sku</t>
+  </si>
   <si>
     <t>name</t>
   </si>
@@ -46,19 +49,28 @@
     <t>meta_title</t>
   </si>
   <si>
-    <t>Yellow dress 1</t>
-  </si>
-  <si>
-    <t>a nice yellow dress</t>
-  </si>
-  <si>
-    <t>Yellow Dress</t>
-  </si>
-  <si>
-    <t>yellow dress</t>
-  </si>
-  <si>
-    <t>Yellglow Dress</t>
+    <t>OPTION=size</t>
+  </si>
+  <si>
+    <t>OPTION=color</t>
+  </si>
+  <si>
+    <t>000000</t>
+  </si>
+  <si>
+    <t>Star Wars t-shirt</t>
+  </si>
+  <si>
+    <t>small, medium, large</t>
+  </si>
+  <si>
+    <t>red, black</t>
+  </si>
+  <si>
+    <t>Terminator t-shirt</t>
+  </si>
+  <si>
+    <t>Metallica t-shirt</t>
   </si>
 </sst>
 </file>
@@ -138,7 +150,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -296,13 +308,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -392,19 +398,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -659,13 +665,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -969,19 +969,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1232,14 +1232,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="12.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11.7578" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1719" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
@@ -1249,7 +1249,10 @@
     <col min="9" max="9" width="10" style="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="1" customWidth="1"/>
-    <col min="12" max="256" width="8.85156" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="1" customWidth="1"/>
+    <col min="15" max="256" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1286,133 +1289,93 @@
       <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
+      <c r="L1" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s" s="2">
-        <v>14</v>
-      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" t="s" s="2">
-        <v>15</v>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s" s="2">
+        <v>17</v>
       </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
       <c r="K3" s="3"/>
+      <c r="L3" s="2"/>
+      <c r="M3" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="A4" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
       <c r="K4" s="3"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="L4" s="2"/>
+      <c r="M4" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="N4" t="s" s="2">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>